<commit_message>
Commit changes to a data file.
</commit_message>
<xml_diff>
--- a/FEBDAQMULTx2/data_analysis/9_utokyo_comparison/data/20210527_second_meeting/mppc_summary_lsu_pcb_lsu_measurements.xlsx
+++ b/FEBDAQMULTx2/data_analysis/9_utokyo_comparison/data/20210527_second_meeting/mppc_summary_lsu_pcb_lsu_measurements.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">position no.</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t xml:space="preserve">MPPC Gain @ over_voltage=5V|Temp=20C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncalibrated Gain @ bias_voltage=57V|Temp=20C</t>
   </si>
   <si>
     <t xml:space="preserve">Noise Rate @ bias_voltage=57V|Temp=25C</t>
@@ -712,11 +715,12 @@
     <col bestFit="1" customWidth="1" min="4" max="4" width="15.42578125"/>
     <col bestFit="1" customWidth="1" min="5" max="6" width="20.28515625"/>
     <col bestFit="1" customWidth="1" min="7" max="8" width="19.28515625"/>
-    <col bestFit="1" customWidth="1" min="9" max="9" width="28.7109375"/>
-    <col bestFit="1" customWidth="1" min="10" max="10" width="26.140625"/>
-    <col bestFit="1" customWidth="1" min="11" max="11" width="16"/>
-    <col bestFit="1" customWidth="1" min="12" max="12" width="20"/>
-    <col bestFit="1" customWidth="1" min="14" max="14" width="36.28515625"/>
+    <col customWidth="1" min="9" max="9" width="19.28515625"/>
+    <col bestFit="1" customWidth="1" min="10" max="10" width="28.7109375"/>
+    <col bestFit="1" customWidth="1" min="11" max="11" width="26.140625"/>
+    <col bestFit="1" customWidth="1" min="12" max="12" width="16"/>
+    <col bestFit="1" customWidth="1" min="13" max="13" width="20"/>
+    <col bestFit="1" customWidth="1" min="15" max="15" width="36.28515625"/>
   </cols>
   <sheetData>
     <row r="1" ht="51" customHeight="1">
@@ -750,20 +754,23 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="P1" t="s">
         <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" ht="14.25">
@@ -771,7 +778,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>51.960000000000001</v>
@@ -783,29 +790,32 @@
         <v>53.640000000000001</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F65" si="0">E2*N2</f>
+        <f>E2*O2</f>
         <v>644702.37839999993</v>
       </c>
       <c r="G2">
         <v>52.850000000000001</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H65" si="1">G2*N2</f>
+        <f>G2*O2</f>
         <v>635207.321</v>
       </c>
-      <c r="J2">
+      <c r="I2">
+        <v>54.250895527158093</v>
+      </c>
+      <c r="K2">
         <v>1863.8499999999999</v>
       </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
       <c r="L2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="4">
+        <v>17</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="4">
         <v>12019.059999999999</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0.1047852851262647</v>
       </c>
     </row>
@@ -814,7 +824,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>51.93</v>
@@ -826,29 +836,32 @@
         <v>52.829999999999998</v>
       </c>
       <c r="F3">
-        <f t="shared" si="0"/>
+        <f>E3*O3</f>
         <v>633131.09729999991</v>
       </c>
       <c r="G3">
         <v>53.039999999999999</v>
       </c>
       <c r="H3">
-        <f t="shared" si="1"/>
+        <f>G3*O3</f>
         <v>635647.80239999993</v>
       </c>
-      <c r="J3">
+      <c r="I3">
+        <v>53.405813968441066</v>
+      </c>
+      <c r="K3">
         <v>1973.3599999999999</v>
       </c>
-      <c r="K3" t="s">
-        <v>16</v>
-      </c>
       <c r="L3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="5">
+        <v>17</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="5">
         <v>11984.309999999999</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0.065167829242769607</v>
       </c>
     </row>
@@ -857,7 +870,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>51.939999999999998</v>
@@ -869,29 +882,32 @@
         <v>55.009999999999998</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f>E4*O4</f>
         <v>660970.45459999994</v>
       </c>
       <c r="G4">
         <v>53.829999999999998</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f>G4*O4</f>
         <v>646792.21179999993</v>
       </c>
-      <c r="J4">
+      <c r="I4">
+        <v>55.693284810051921</v>
+      </c>
+      <c r="K4">
         <v>2331.73</v>
       </c>
-      <c r="K4" t="s">
-        <v>16</v>
-      </c>
       <c r="L4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="5">
+        <v>17</v>
+      </c>
+      <c r="M4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="5">
         <v>12015.459999999999</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>0.075326954782795802</v>
       </c>
     </row>
@@ -900,7 +916,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>51.969999999999999</v>
@@ -912,29 +928,32 @@
         <v>53.880000000000003</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f>E5*O5</f>
         <v>648625.22039999999</v>
       </c>
       <c r="G5">
         <v>53.729999999999997</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
+        <f>G5*O5</f>
         <v>646819.47089999996</v>
       </c>
-      <c r="J5">
+      <c r="I5">
+        <v>53.569186385896906</v>
+      </c>
+      <c r="K5">
         <v>1808.8299999999999</v>
       </c>
-      <c r="K5" t="s">
-        <v>16</v>
-      </c>
       <c r="L5" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" s="5">
+        <v>17</v>
+      </c>
+      <c r="M5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="5">
         <v>12038.33</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>0.085310698013314895</v>
       </c>
     </row>
@@ -943,7 +962,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>51.609999999999999</v>
@@ -955,29 +974,32 @@
         <v>51.219999999999999</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f>E6*O6</f>
         <v>622329.65859999997</v>
       </c>
       <c r="G6">
         <v>51.159999999999997</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
+        <f>G6*O6</f>
         <v>621600.65079999994</v>
       </c>
-      <c r="J6">
+      <c r="I6">
+        <v>54.970971010845446</v>
+      </c>
+      <c r="K6">
         <v>2762.3600000000001</v>
       </c>
-      <c r="K6" t="s">
-        <v>16</v>
-      </c>
       <c r="L6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" s="5">
+        <v>17</v>
+      </c>
+      <c r="M6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="5">
         <v>12150.129999999999</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>0.052262130339370202</v>
       </c>
     </row>
@@ -986,7 +1008,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>51.640000000000001</v>
@@ -998,29 +1020,32 @@
         <v>51.609999999999999</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f>E7*O7</f>
         <v>617700.47820000001</v>
       </c>
       <c r="G7">
         <v>52.219999999999999</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
+        <f>G7*O7</f>
         <v>625001.33640000003</v>
       </c>
-      <c r="J7">
+      <c r="I7">
+        <v>54.629679136898083</v>
+      </c>
+      <c r="K7">
         <v>1895.49</v>
       </c>
-      <c r="K7" t="s">
-        <v>16</v>
-      </c>
       <c r="L7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N7" s="5">
+        <v>17</v>
+      </c>
+      <c r="M7" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="5">
         <v>11968.620000000001</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>0.037734303981825097</v>
       </c>
     </row>
@@ -1029,7 +1054,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>51.799999999999997</v>
@@ -1041,29 +1066,32 @@
         <v>53.619999999999997</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f>E8*O8</f>
         <v>646531.19299999997</v>
       </c>
       <c r="G8">
         <v>52.299999999999997</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
+        <f>G8*O8</f>
         <v>630615.09499999997</v>
       </c>
-      <c r="J8" t="s">
-        <v>17</v>
+      <c r="I8">
+        <v>56.154906726503192</v>
       </c>
       <c r="K8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L8" t="s">
-        <v>16</v>
-      </c>
-      <c r="N8" s="5">
+        <v>17</v>
+      </c>
+      <c r="M8" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="5">
         <v>12057.65</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>0.048697525156839297</v>
       </c>
     </row>
@@ -1072,7 +1100,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>51.780000000000001</v>
@@ -1084,29 +1112,32 @@
         <v>53.270000000000003</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f>E9*O9</f>
         <v>639661.36570000008</v>
       </c>
       <c r="G9">
         <v>52.670000000000002</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f>G9*O9</f>
         <v>632456.61970000004</v>
       </c>
-      <c r="J9">
+      <c r="I9">
+        <v>55.885678229301298</v>
+      </c>
+      <c r="K9">
         <v>2110.2800000000002</v>
       </c>
-      <c r="K9" t="s">
-        <v>16</v>
-      </c>
       <c r="L9" t="s">
-        <v>16</v>
-      </c>
-      <c r="N9" s="5">
+        <v>17</v>
+      </c>
+      <c r="M9" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9" s="5">
         <v>12007.91</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>0.074750198746735996</v>
       </c>
     </row>
@@ -1115,7 +1146,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>52.100000000000001</v>
@@ -1127,29 +1158,32 @@
         <v>56.25</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f>E10*O10</f>
         <v>669406.5</v>
       </c>
       <c r="G10">
         <v>53.520000000000003</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
+        <f>G10*O10</f>
         <v>636917.97120000003</v>
       </c>
-      <c r="J10">
+      <c r="I10">
+        <v>55.62654823717213</v>
+      </c>
+      <c r="K10">
         <v>2903.6900000000001</v>
       </c>
-      <c r="K10" t="s">
-        <v>16</v>
-      </c>
       <c r="L10" t="s">
-        <v>16</v>
-      </c>
-      <c r="N10" s="5">
+        <v>17</v>
+      </c>
+      <c r="M10" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" s="5">
         <v>11900.559999999999</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>0.067059197548611199</v>
       </c>
     </row>
@@ -1158,7 +1192,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>52</v>
@@ -1170,29 +1204,32 @@
         <v>53.479999999999997</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f>E11*O11</f>
         <v>643239.25679999997</v>
       </c>
       <c r="G11">
         <v>53.450000000000003</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
+        <f>G11*O11</f>
         <v>642878.42700000003</v>
       </c>
-      <c r="J11">
+      <c r="I11">
+        <v>53.002419353664536</v>
+      </c>
+      <c r="K11">
         <v>1954.01</v>
       </c>
-      <c r="K11" t="s">
-        <v>16</v>
-      </c>
       <c r="L11" t="s">
-        <v>16</v>
-      </c>
-      <c r="N11" s="5">
+        <v>17</v>
+      </c>
+      <c r="M11" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="5">
         <v>12027.66</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>0.065546995028494606</v>
       </c>
     </row>
@@ -1201,7 +1238,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>51.990000000000002</v>
@@ -1213,29 +1250,32 @@
         <v>55.390000000000001</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f>E12*O12</f>
         <v>661614.71739999996</v>
       </c>
       <c r="G12">
         <v>53.770000000000003</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
+        <f>G12*O12</f>
         <v>642264.36820000003</v>
       </c>
-      <c r="J12">
+      <c r="I12">
+        <v>55.446838313236732</v>
+      </c>
+      <c r="K12">
         <v>2447.8200000000002</v>
       </c>
-      <c r="K12" t="s">
-        <v>16</v>
-      </c>
       <c r="L12" t="s">
-        <v>16</v>
-      </c>
-      <c r="N12" s="5">
+        <v>17</v>
+      </c>
+      <c r="M12" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" s="5">
         <v>11944.66</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>0.053249111536164802</v>
       </c>
     </row>
@@ -1244,7 +1284,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13">
         <v>51.909999999999997</v>
@@ -1256,29 +1296,32 @@
         <v>53.560000000000002</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f>E13*O13</f>
         <v>639474.26399999997</v>
       </c>
       <c r="G13">
         <v>53.789999999999999</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
+        <f>G13*O13</f>
         <v>642220.326</v>
       </c>
-      <c r="J13">
+      <c r="I13">
+        <v>54.315263605202176</v>
+      </c>
+      <c r="K13">
         <v>1771.04</v>
       </c>
-      <c r="K13" t="s">
-        <v>16</v>
-      </c>
       <c r="L13" t="s">
-        <v>16</v>
-      </c>
-      <c r="N13" s="5">
+        <v>17</v>
+      </c>
+      <c r="M13" t="s">
+        <v>17</v>
+      </c>
+      <c r="O13" s="5">
         <v>11939.4</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>0.052652956268821501</v>
       </c>
     </row>
@@ -1287,7 +1330,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C14">
         <v>51.829999999999998</v>
@@ -1299,29 +1342,32 @@
         <v>53.200000000000003</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f>E14*O14</f>
         <v>634716.96400000004</v>
       </c>
       <c r="G14">
         <v>52.390000000000001</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
+        <f>G14*O14</f>
         <v>625053.04029999999</v>
       </c>
-      <c r="J14">
+      <c r="I14">
+        <v>54.952676813702723</v>
+      </c>
+      <c r="K14">
         <v>1669.3599999999999</v>
       </c>
-      <c r="K14" t="s">
-        <v>16</v>
-      </c>
       <c r="L14" t="s">
-        <v>16</v>
-      </c>
-      <c r="N14" s="5">
+        <v>17</v>
+      </c>
+      <c r="M14" t="s">
+        <v>17</v>
+      </c>
+      <c r="O14" s="5">
         <v>11930.77</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>0.047726232240233701</v>
       </c>
     </row>
@@ -1330,7 +1376,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>51.899999999999999</v>
@@ -1342,29 +1388,32 @@
         <v>54.439999999999998</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f>E15*O15</f>
         <v>655357.43039999995</v>
       </c>
       <c r="G15">
         <v>55.140000000000001</v>
       </c>
       <c r="H15">
-        <f t="shared" si="1"/>
+        <f>G15*O15</f>
         <v>663784.14240000001</v>
       </c>
-      <c r="J15">
+      <c r="I15">
+        <v>55.521761042666462</v>
+      </c>
+      <c r="K15">
         <v>1609.74</v>
       </c>
-      <c r="K15" t="s">
-        <v>16</v>
-      </c>
       <c r="L15" t="s">
-        <v>16</v>
-      </c>
-      <c r="N15" s="5">
+        <v>17</v>
+      </c>
+      <c r="M15" t="s">
+        <v>17</v>
+      </c>
+      <c r="O15" s="5">
         <v>12038.16</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>0.0644232971255006</v>
       </c>
     </row>
@@ -1373,7 +1422,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>51.909999999999997</v>
@@ -1385,29 +1434,32 @@
         <v>53.75</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f>E16*O16</f>
         <v>641597.08750000002</v>
       </c>
       <c r="G16">
         <v>55.740000000000002</v>
       </c>
       <c r="H16">
-        <f t="shared" si="1"/>
+        <f>G16*O16</f>
         <v>665351.10060000001</v>
       </c>
-      <c r="J16">
+      <c r="I16">
+        <v>54.527388424593397</v>
+      </c>
+      <c r="K16">
         <v>1974.4000000000001</v>
       </c>
-      <c r="K16" t="s">
-        <v>16</v>
-      </c>
       <c r="L16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N16" s="5">
+        <v>17</v>
+      </c>
+      <c r="M16" t="s">
+        <v>17</v>
+      </c>
+      <c r="O16" s="5">
         <v>11936.690000000001</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>0.039154989327744603</v>
       </c>
     </row>
@@ -1416,7 +1468,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17">
         <v>51.890000000000001</v>
@@ -1428,29 +1480,32 @@
         <v>53.969999999999999</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f>E17*O17</f>
         <v>634579.79969999997</v>
       </c>
       <c r="G17">
         <v>56.380000000000003</v>
       </c>
       <c r="H17">
-        <f t="shared" si="1"/>
+        <f>G17*O17</f>
         <v>662916.60380000004</v>
       </c>
-      <c r="J17">
+      <c r="I17">
+        <v>54.428836562429794</v>
+      </c>
+      <c r="K17">
         <v>4995.6000000000004</v>
       </c>
-      <c r="K17" t="s">
-        <v>16</v>
-      </c>
       <c r="L17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N17" s="5">
+        <v>17</v>
+      </c>
+      <c r="M17" t="s">
+        <v>17</v>
+      </c>
+      <c r="O17" s="5">
         <v>11758.01</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>0.064723551024785206</v>
       </c>
     </row>
@@ -1459,7 +1514,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18">
         <v>52.090000000000003</v>
@@ -1471,29 +1526,32 @@
         <v>54.920000000000002</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f>E18*O18</f>
         <v>643967.75520000001</v>
       </c>
       <c r="G18">
         <v>50.859999999999999</v>
       </c>
       <c r="H18">
-        <f t="shared" si="1"/>
+        <f>G18*O18</f>
         <v>596361.98159999994</v>
       </c>
-      <c r="J18">
+      <c r="I18">
+        <v>54.07361334106308</v>
+      </c>
+      <c r="K18">
         <v>2475.6700000000001</v>
       </c>
-      <c r="K18" t="s">
-        <v>16</v>
-      </c>
       <c r="L18" t="s">
-        <v>16</v>
-      </c>
-      <c r="N18" s="5">
+        <v>17</v>
+      </c>
+      <c r="M18" t="s">
+        <v>17</v>
+      </c>
+      <c r="O18" s="5">
         <v>11725.559999999999</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>0</v>
       </c>
     </row>
@@ -1502,7 +1560,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19">
         <v>52.090000000000003</v>
@@ -1514,29 +1572,32 @@
         <v>53.689999999999998</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f>E19*O19</f>
         <v>646958.05719999992</v>
       </c>
       <c r="G19">
         <v>53.439999999999998</v>
       </c>
       <c r="H19">
-        <f t="shared" si="1"/>
+        <f>G19*O19</f>
         <v>643945.58719999995</v>
       </c>
-      <c r="J19">
+      <c r="I19">
+        <v>52.527298043733865</v>
+      </c>
+      <c r="K19">
         <v>2182.8600000000001</v>
       </c>
-      <c r="K19" t="s">
-        <v>16</v>
-      </c>
       <c r="L19" t="s">
-        <v>16</v>
-      </c>
-      <c r="N19" s="5">
+        <v>17</v>
+      </c>
+      <c r="M19" t="s">
+        <v>17</v>
+      </c>
+      <c r="O19" s="5">
         <v>12049.879999999999</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>0.051616899976762401</v>
       </c>
     </row>
@@ -1545,7 +1606,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C20">
         <v>52.030000000000001</v>
@@ -1557,29 +1618,32 @@
         <v>55.310000000000002</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f>E20*O20</f>
         <v>664983.28040000005</v>
       </c>
       <c r="G20">
         <v>55.390000000000001</v>
       </c>
       <c r="H20">
-        <f t="shared" si="1"/>
+        <f>G20*O20</f>
         <v>665945.10759999999</v>
       </c>
-      <c r="J20">
+      <c r="I20">
+        <v>54.518329111128473</v>
+      </c>
+      <c r="K20">
         <v>1890.28</v>
       </c>
-      <c r="K20" t="s">
-        <v>16</v>
-      </c>
       <c r="L20" t="s">
-        <v>16</v>
-      </c>
-      <c r="N20" s="5">
+        <v>17</v>
+      </c>
+      <c r="M20" t="s">
+        <v>17</v>
+      </c>
+      <c r="O20" s="5">
         <v>12022.84</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>0.050430776085064001</v>
       </c>
     </row>
@@ -1588,7 +1652,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21">
         <v>52.100000000000001</v>
@@ -1600,29 +1664,32 @@
         <v>54.789999999999999</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
+        <f>E21*O21</f>
         <v>664630.09499999997</v>
       </c>
       <c r="G21">
         <v>54.829999999999998</v>
       </c>
       <c r="H21">
-        <f t="shared" si="1"/>
+        <f>G21*O21</f>
         <v>665115.31499999994</v>
       </c>
-      <c r="J21">
+      <c r="I21">
+        <v>53.725117097206684</v>
+      </c>
+      <c r="K21">
         <v>2655.2199999999998</v>
       </c>
-      <c r="K21" t="s">
-        <v>16</v>
-      </c>
       <c r="L21" t="s">
-        <v>16</v>
-      </c>
-      <c r="N21" s="5">
+        <v>17</v>
+      </c>
+      <c r="M21" t="s">
+        <v>17</v>
+      </c>
+      <c r="O21" s="5">
         <v>12130.5</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>0.041905577811777103</v>
       </c>
     </row>
@@ -1631,7 +1698,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C22">
         <v>51.850000000000001</v>
@@ -1643,29 +1710,32 @@
         <v>53.350000000000001</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f>E22*O22</f>
         <v>643081.96700000006</v>
       </c>
       <c r="G22">
         <v>56.770000000000003</v>
       </c>
       <c r="H22">
-        <f t="shared" si="1"/>
+        <f>G22*O22</f>
         <v>684306.7154000001</v>
       </c>
-      <c r="J22">
+      <c r="I22">
+        <v>53.923285573759202</v>
+      </c>
+      <c r="K22">
         <v>2719.6900000000001</v>
       </c>
-      <c r="K22" t="s">
-        <v>16</v>
-      </c>
       <c r="L22" t="s">
-        <v>16</v>
-      </c>
-      <c r="N22" s="5">
+        <v>17</v>
+      </c>
+      <c r="M22" t="s">
+        <v>17</v>
+      </c>
+      <c r="O22" s="5">
         <v>12054.02</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>0.094434976459276704</v>
       </c>
     </row>
@@ -1674,7 +1744,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C23">
         <v>52.079999999999998</v>
@@ -1686,29 +1756,32 @@
         <v>55.090000000000003</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f>E23*O23</f>
         <v>651198.50670000003</v>
       </c>
       <c r="G23">
         <v>53.539999999999999</v>
       </c>
       <c r="H23">
-        <f t="shared" si="1"/>
+        <f>G23*O23</f>
         <v>632876.53019999992</v>
       </c>
-      <c r="J23">
+      <c r="I23">
+        <v>53.952380809683987</v>
+      </c>
+      <c r="K23">
         <v>2030.3399999999999</v>
       </c>
-      <c r="K23" t="s">
-        <v>16</v>
-      </c>
       <c r="L23" t="s">
-        <v>16</v>
-      </c>
-      <c r="N23" s="5">
+        <v>17</v>
+      </c>
+      <c r="M23" t="s">
+        <v>17</v>
+      </c>
+      <c r="O23" s="5">
         <v>11820.629999999999</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>0.0726143835241993</v>
       </c>
     </row>
@@ -1717,7 +1790,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C24">
         <v>52</v>
@@ -1729,29 +1802,32 @@
         <v>55.130000000000003</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f>E24*O24</f>
         <v>649590.17440000002</v>
       </c>
       <c r="G24">
         <v>53.670000000000002</v>
       </c>
       <c r="H24">
-        <f t="shared" si="1"/>
+        <f>G24*O24</f>
         <v>632387.16960000002</v>
       </c>
-      <c r="J24">
+      <c r="I24">
+        <v>54.936944951775246</v>
+      </c>
+      <c r="K24">
         <v>2181.6999999999998</v>
       </c>
-      <c r="K24" t="s">
-        <v>16</v>
-      </c>
       <c r="L24" t="s">
-        <v>16</v>
-      </c>
-      <c r="N24" s="5">
+        <v>17</v>
+      </c>
+      <c r="M24" t="s">
+        <v>17</v>
+      </c>
+      <c r="O24" s="5">
         <v>11782.879999999999</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>0.066745167113213003</v>
       </c>
     </row>
@@ -1760,7 +1836,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C25">
         <v>51.93</v>
@@ -1772,29 +1848,32 @@
         <v>54.450000000000003</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
+        <f>E25*O25</f>
         <v>658398.51000000001</v>
       </c>
       <c r="G25">
         <v>54.770000000000003</v>
       </c>
       <c r="H25">
-        <f t="shared" si="1"/>
+        <f>G25*O25</f>
         <v>662267.88599999994</v>
       </c>
-      <c r="J25">
+      <c r="I25">
+        <v>54.921038488463566</v>
+      </c>
+      <c r="K25">
         <v>4424.2399999999998</v>
       </c>
-      <c r="K25" t="s">
-        <v>16</v>
-      </c>
       <c r="L25" t="s">
-        <v>16</v>
-      </c>
-      <c r="N25" s="5">
+        <v>17</v>
+      </c>
+      <c r="M25" t="s">
+        <v>17</v>
+      </c>
+      <c r="O25" s="5">
         <v>12091.799999999999</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>0.093755365072286406</v>
       </c>
     </row>
@@ -1803,7 +1882,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C26">
         <v>51.950000000000003</v>
@@ -1815,29 +1894,32 @@
         <v>54.969999999999999</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
+        <f>E26*O26</f>
         <v>660971.37339999992</v>
       </c>
       <c r="G26">
         <v>50.109999999999999</v>
       </c>
       <c r="H26">
-        <f t="shared" si="1"/>
+        <f>G26*O26</f>
         <v>602533.6642</v>
       </c>
-      <c r="J26">
+      <c r="I26">
+        <v>55.307326970333335</v>
+      </c>
+      <c r="K26">
         <v>1965.9000000000001</v>
       </c>
-      <c r="K26" t="s">
-        <v>16</v>
-      </c>
       <c r="L26" t="s">
-        <v>16</v>
-      </c>
-      <c r="N26" s="5">
+        <v>17</v>
+      </c>
+      <c r="M26" t="s">
+        <v>17</v>
+      </c>
+      <c r="O26" s="5">
         <v>12024.219999999999</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>0.028451233772938001</v>
       </c>
     </row>
@@ -1846,7 +1928,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C27">
         <v>52.130000000000003</v>
@@ -1858,29 +1940,32 @@
         <v>56.909999999999997</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
+        <f>E27*O27</f>
         <v>673762.61190000002</v>
       </c>
       <c r="G27">
         <v>53.109999999999999</v>
       </c>
       <c r="H27">
-        <f t="shared" si="1"/>
+        <f>G27*O27</f>
         <v>628774.0699</v>
       </c>
-      <c r="J27">
+      <c r="I27">
+        <v>55.403850745485848</v>
+      </c>
+      <c r="K27">
         <v>2490.7199999999998</v>
       </c>
-      <c r="K27" t="s">
-        <v>16</v>
-      </c>
       <c r="L27" t="s">
-        <v>16</v>
-      </c>
-      <c r="N27" s="5">
+        <v>17</v>
+      </c>
+      <c r="M27" t="s">
+        <v>17</v>
+      </c>
+      <c r="O27" s="5">
         <v>11839.09</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>0.086985091468272296</v>
       </c>
     </row>
@@ -1889,7 +1974,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C28">
         <v>52.229999999999997</v>
@@ -1901,29 +1986,32 @@
         <v>57.579999999999998</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
+        <f>E28*O28</f>
         <v>689084.61939999997</v>
       </c>
       <c r="G28">
         <v>55.659999999999997</v>
       </c>
       <c r="H28">
-        <f t="shared" si="1"/>
+        <f>G28*O28</f>
         <v>666107.15379999997</v>
       </c>
-      <c r="J28">
+      <c r="I28">
+        <v>54.813693770313897</v>
+      </c>
+      <c r="K28">
         <v>2022.29</v>
       </c>
-      <c r="K28" t="s">
-        <v>16</v>
-      </c>
       <c r="L28" t="s">
-        <v>16</v>
-      </c>
-      <c r="N28" s="5">
+        <v>17</v>
+      </c>
+      <c r="M28" t="s">
+        <v>17</v>
+      </c>
+      <c r="O28" s="5">
         <v>11967.43</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>0.062986654345636606</v>
       </c>
     </row>
@@ -1932,7 +2020,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C29">
         <v>52.030000000000001</v>
@@ -1944,29 +2032,32 @@
         <v>56.710000000000001</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
+        <f>E29*O29</f>
         <v>683564.19280000008</v>
       </c>
       <c r="G29">
         <v>54.590000000000003</v>
       </c>
       <c r="H29">
-        <f t="shared" si="1"/>
+        <f>G29*O29</f>
         <v>658010.39120000007</v>
       </c>
-      <c r="J29">
+      <c r="I29">
+        <v>56.334950964547723</v>
+      </c>
+      <c r="K29">
         <v>1807.28</v>
       </c>
-      <c r="K29" t="s">
-        <v>16</v>
-      </c>
       <c r="L29" t="s">
-        <v>16</v>
-      </c>
-      <c r="N29" s="5">
+        <v>17</v>
+      </c>
+      <c r="M29" t="s">
+        <v>17</v>
+      </c>
+      <c r="O29" s="5">
         <v>12053.68</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <v>0.043049259827035703</v>
       </c>
     </row>
@@ -1975,7 +2066,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C30">
         <v>52.18</v>
@@ -1987,29 +2078,32 @@
         <v>55.149999999999999</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
+        <f>E30*O30</f>
         <v>661886.58549999993</v>
       </c>
       <c r="G30">
         <v>52.200000000000003</v>
       </c>
       <c r="H30">
-        <f t="shared" si="1"/>
+        <f>G30*O30</f>
         <v>626481.95400000003</v>
       </c>
-      <c r="J30">
+      <c r="I30">
+        <v>53.287661670889534</v>
+      </c>
+      <c r="K30">
         <v>2493.1799999999998</v>
       </c>
-      <c r="K30" t="s">
-        <v>16</v>
-      </c>
       <c r="L30" t="s">
-        <v>16</v>
-      </c>
-      <c r="N30" s="5">
+        <v>17</v>
+      </c>
+      <c r="M30" t="s">
+        <v>17</v>
+      </c>
+      <c r="O30" s="5">
         <v>12001.57</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <v>0.106254642518294</v>
       </c>
     </row>
@@ -2018,7 +2112,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C31">
         <v>52.149999999999999</v>
@@ -2030,29 +2124,32 @@
         <v>56.219999999999999</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
+        <f>E31*O31</f>
         <v>684583.06920000003</v>
       </c>
       <c r="G31">
         <v>53.100000000000001</v>
       </c>
       <c r="H31">
-        <f t="shared" si="1"/>
+        <f>G31*O31</f>
         <v>646591.26600000006</v>
       </c>
-      <c r="J31">
+      <c r="I31">
+        <v>54.887151239206048</v>
+      </c>
+      <c r="K31">
         <v>1734.79</v>
       </c>
-      <c r="K31" t="s">
-        <v>16</v>
-      </c>
       <c r="L31" t="s">
-        <v>16</v>
-      </c>
-      <c r="N31" s="5">
+        <v>17</v>
+      </c>
+      <c r="M31" t="s">
+        <v>17</v>
+      </c>
+      <c r="O31" s="5">
         <v>12176.860000000001</v>
       </c>
-      <c r="O31">
+      <c r="P31">
         <v>0.099514408108733104</v>
       </c>
     </row>
@@ -2061,7 +2158,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C32">
         <v>51.609999999999999</v>
@@ -2073,29 +2170,32 @@
         <v>51.640000000000001</v>
       </c>
       <c r="F32">
-        <f t="shared" si="0"/>
+        <f>E32*O32</f>
         <v>619187.35439999995</v>
       </c>
       <c r="G32">
         <v>54.82</v>
       </c>
       <c r="H32">
-        <f t="shared" si="1"/>
+        <f>G32*O32</f>
         <v>657317.0172</v>
       </c>
-      <c r="J32">
+      <c r="I32">
+        <v>55.09362110605921</v>
+      </c>
+      <c r="K32">
         <v>1646.4300000000001</v>
       </c>
-      <c r="K32" t="s">
-        <v>16</v>
-      </c>
       <c r="L32" t="s">
-        <v>16</v>
-      </c>
-      <c r="N32" s="5">
+        <v>17</v>
+      </c>
+      <c r="M32" t="s">
+        <v>17</v>
+      </c>
+      <c r="O32" s="5">
         <v>11990.459999999999</v>
       </c>
-      <c r="O32">
+      <c r="P32">
         <v>0.076183610475607594</v>
       </c>
     </row>
@@ -2104,7 +2204,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C33">
         <v>51.939999999999998</v>
@@ -2116,29 +2216,32 @@
         <v>53.670000000000002</v>
       </c>
       <c r="F33">
-        <f t="shared" si="0"/>
+        <f>E33*O33</f>
         <v>650846.96609999996</v>
       </c>
       <c r="G33">
         <v>56.359999999999999</v>
       </c>
       <c r="H33">
-        <f t="shared" si="1"/>
+        <f>G33*O33</f>
         <v>683468.13879999996</v>
       </c>
-      <c r="J33">
+      <c r="I33">
+        <v>54.3158015724308</v>
+      </c>
+      <c r="K33">
         <v>1820.52</v>
       </c>
-      <c r="K33" t="s">
-        <v>16</v>
-      </c>
       <c r="L33" t="s">
-        <v>16</v>
-      </c>
-      <c r="N33" s="6">
+        <v>17</v>
+      </c>
+      <c r="M33" t="s">
+        <v>17</v>
+      </c>
+      <c r="O33" s="6">
         <v>12126.83</v>
       </c>
-      <c r="O33">
+      <c r="P33">
         <v>0.057240302468436997</v>
       </c>
     </row>
@@ -2147,7 +2250,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C34">
         <v>52.310000000000002</v>
@@ -2159,29 +2262,32 @@
         <v>51.380000000000003</v>
       </c>
       <c r="F34">
-        <f t="shared" si="0"/>
+        <f>E34*O34</f>
         <v>617539.30279999995</v>
       </c>
       <c r="G34">
         <v>54.479999999999997</v>
       </c>
       <c r="H34">
-        <f t="shared" si="1"/>
+        <f>G34*O34</f>
         <v>654798.38879999996</v>
       </c>
-      <c r="J34">
+      <c r="I34">
+        <v>53.475072195142097</v>
+      </c>
+      <c r="K34">
         <v>1645.03</v>
       </c>
-      <c r="K34" t="s">
-        <v>16</v>
-      </c>
       <c r="L34" t="s">
-        <v>16</v>
-      </c>
-      <c r="N34" s="4">
+        <v>17</v>
+      </c>
+      <c r="M34" t="s">
+        <v>17</v>
+      </c>
+      <c r="O34" s="4">
         <v>12019.059999999999</v>
       </c>
-      <c r="O34">
+      <c r="P34">
         <v>0.18171509349530349</v>
       </c>
     </row>
@@ -2190,7 +2296,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C35">
         <v>51.869999999999997</v>
@@ -2202,29 +2308,32 @@
         <v>48.549999999999997</v>
       </c>
       <c r="F35">
-        <f t="shared" si="0"/>
+        <f>E35*O35</f>
         <v>581838.25049999997</v>
       </c>
       <c r="G35">
         <v>51.780000000000001</v>
       </c>
       <c r="H35">
-        <f t="shared" si="1"/>
+        <f>G35*O35</f>
         <v>620547.57180000003</v>
       </c>
-      <c r="J35">
+      <c r="I35">
+        <v>53.210000292647685</v>
+      </c>
+      <c r="K35">
         <v>1602.49</v>
       </c>
-      <c r="K35" t="s">
-        <v>16</v>
-      </c>
       <c r="L35" t="s">
-        <v>16</v>
-      </c>
-      <c r="N35" s="5">
+        <v>17</v>
+      </c>
+      <c r="M35" t="s">
+        <v>17</v>
+      </c>
+      <c r="O35" s="5">
         <v>11984.309999999999</v>
       </c>
-      <c r="O35">
+      <c r="P35">
         <v>0.35169454991058402</v>
       </c>
     </row>
@@ -2233,7 +2342,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C36">
         <v>51.82</v>
@@ -2245,29 +2354,32 @@
         <v>49.880000000000003</v>
       </c>
       <c r="F36">
-        <f t="shared" si="0"/>
+        <f>E36*O36</f>
         <v>599331.14480000001</v>
       </c>
       <c r="G36">
         <v>53.520000000000003</v>
       </c>
       <c r="H36">
-        <f t="shared" si="1"/>
+        <f>G36*O36</f>
         <v>643067.4192</v>
       </c>
-      <c r="J36">
+      <c r="I36">
+        <v>54.754846222486783</v>
+      </c>
+      <c r="K36">
         <v>1593.0999999999999</v>
       </c>
-      <c r="K36" t="s">
-        <v>16</v>
-      </c>
       <c r="L36" t="s">
-        <v>16</v>
-      </c>
-      <c r="N36" s="5">
+        <v>17</v>
+      </c>
+      <c r="M36" t="s">
+        <v>17</v>
+      </c>
+      <c r="O36" s="5">
         <v>12015.459999999999</v>
       </c>
-      <c r="O36">
+      <c r="P36">
         <v>0.086724403152576401</v>
       </c>
     </row>
@@ -2276,7 +2388,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C37">
         <v>51.600000000000001</v>
@@ -2288,26 +2400,29 @@
         <v>47.149999999999999</v>
       </c>
       <c r="F37">
-        <f t="shared" si="0"/>
+        <f>E37*O37</f>
         <v>567607.25949999993</v>
       </c>
       <c r="G37">
         <v>53.109999999999999</v>
       </c>
       <c r="H37">
-        <f t="shared" si="1"/>
+        <f>G37*O37</f>
         <v>639355.70629999996</v>
       </c>
-      <c r="K37" t="s">
-        <v>16</v>
+      <c r="I37">
+        <v>53.342458206849599</v>
       </c>
       <c r="L37" t="s">
-        <v>16</v>
-      </c>
-      <c r="N37" s="5">
+        <v>17</v>
+      </c>
+      <c r="M37" t="s">
+        <v>17</v>
+      </c>
+      <c r="O37" s="5">
         <v>12038.33</v>
       </c>
-      <c r="O37">
+      <c r="P37">
         <v>0.57387236280668052</v>
       </c>
     </row>
@@ -2316,7 +2431,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C38">
         <v>51.659999999999997</v>
@@ -2328,29 +2443,32 @@
         <v>46.909999999999997</v>
       </c>
       <c r="F38">
-        <f t="shared" si="0"/>
+        <f>E38*O38</f>
         <v>569962.59829999995</v>
       </c>
       <c r="G38">
         <v>50.850000000000001</v>
       </c>
       <c r="H38">
-        <f t="shared" si="1"/>
+        <f>G38*O38</f>
         <v>617834.11049999995</v>
       </c>
-      <c r="J38">
+      <c r="I38">
+        <v>51.318233564978762</v>
+      </c>
+      <c r="K38">
         <v>1891.27</v>
       </c>
-      <c r="K38" t="s">
-        <v>16</v>
-      </c>
       <c r="L38" t="s">
-        <v>16</v>
-      </c>
-      <c r="N38" s="5">
+        <v>17</v>
+      </c>
+      <c r="M38" t="s">
+        <v>17</v>
+      </c>
+      <c r="O38" s="5">
         <v>12150.129999999999</v>
       </c>
-      <c r="O38">
+      <c r="P38">
         <v>0.34767716886938371</v>
       </c>
     </row>
@@ -2359,7 +2477,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C39">
         <v>51.700000000000003</v>
@@ -2371,26 +2489,29 @@
         <v>46.530000000000001</v>
       </c>
       <c r="F39">
-        <f t="shared" si="0"/>
+        <f>E39*O39</f>
         <v>556899.88860000006</v>
       </c>
       <c r="G39">
         <v>50.979999999999997</v>
       </c>
       <c r="H39">
-        <f t="shared" si="1"/>
+        <f>G39*O39</f>
         <v>610160.2476</v>
       </c>
-      <c r="K39" t="s">
-        <v>16</v>
+      <c r="I39">
+        <v>50.673855228643582</v>
       </c>
       <c r="L39" t="s">
-        <v>16</v>
-      </c>
-      <c r="N39" s="5">
+        <v>17</v>
+      </c>
+      <c r="M39" t="s">
+        <v>17</v>
+      </c>
+      <c r="O39" s="5">
         <v>11968.620000000001</v>
       </c>
-      <c r="O39">
+      <c r="P39">
         <v>0.0420334845150361</v>
       </c>
     </row>
@@ -2399,7 +2520,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C40">
         <v>52.100000000000001</v>
@@ -2411,26 +2532,29 @@
         <v>50.100000000000001</v>
       </c>
       <c r="F40">
-        <f t="shared" si="0"/>
+        <f>E40*O40</f>
         <v>604088.26500000001</v>
       </c>
       <c r="G40">
         <v>53.090000000000003</v>
       </c>
       <c r="H40">
-        <f t="shared" si="1"/>
+        <f>G40*O40</f>
         <v>640140.6385</v>
       </c>
-      <c r="K40" t="s">
-        <v>16</v>
+      <c r="I40">
+        <v>52.084116149338463</v>
       </c>
       <c r="L40" t="s">
-        <v>16</v>
-      </c>
-      <c r="N40" s="5">
+        <v>17</v>
+      </c>
+      <c r="M40" t="s">
+        <v>17</v>
+      </c>
+      <c r="O40" s="5">
         <v>12057.65</v>
       </c>
-      <c r="O40">
+      <c r="P40">
         <v>0.17556900665044681</v>
       </c>
     </row>
@@ -2439,7 +2563,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C41">
         <v>51.539999999999999</v>
@@ -2451,26 +2575,29 @@
         <v>45.789999999999999</v>
       </c>
       <c r="F41">
-        <f t="shared" si="0"/>
+        <f>E41*O41</f>
         <v>549842.19889999996</v>
       </c>
       <c r="G41">
         <v>52.490000000000002</v>
       </c>
       <c r="H41">
-        <f t="shared" si="1"/>
+        <f>G41*O41</f>
         <v>630295.19590000005</v>
       </c>
-      <c r="K41" t="s">
-        <v>16</v>
+      <c r="I41">
+        <v>54.007792179753601</v>
       </c>
       <c r="L41" t="s">
-        <v>16</v>
-      </c>
-      <c r="N41" s="5">
+        <v>17</v>
+      </c>
+      <c r="M41" t="s">
+        <v>17</v>
+      </c>
+      <c r="O41" s="5">
         <v>12007.91</v>
       </c>
-      <c r="O41">
+      <c r="P41">
         <v>0.081662306253711694</v>
       </c>
     </row>
@@ -2479,7 +2606,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C42">
         <v>51.810000000000002</v>
@@ -2491,29 +2618,32 @@
         <v>47.740000000000002</v>
       </c>
       <c r="F42">
-        <f t="shared" si="0"/>
+        <f>E42*O42</f>
         <v>568132.73439999996</v>
       </c>
       <c r="G42">
         <v>43.450000000000003</v>
       </c>
       <c r="H42">
-        <f t="shared" si="1"/>
+        <f>G42*O42</f>
         <v>517079.33199999999</v>
       </c>
-      <c r="J42">
+      <c r="I42">
+        <v>54.561917566092575</v>
+      </c>
+      <c r="K42">
         <v>1727.6800000000001</v>
       </c>
-      <c r="K42" t="s">
-        <v>16</v>
-      </c>
       <c r="L42" t="s">
-        <v>16</v>
-      </c>
-      <c r="N42" s="5">
+        <v>17</v>
+      </c>
+      <c r="M42" t="s">
+        <v>17</v>
+      </c>
+      <c r="O42" s="5">
         <v>11900.559999999999</v>
       </c>
-      <c r="O42">
+      <c r="P42">
         <v>0.071754693605725298</v>
       </c>
     </row>
@@ -2522,7 +2652,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C43">
         <v>52.390000000000001</v>
@@ -2534,26 +2664,29 @@
         <v>51.700000000000003</v>
       </c>
       <c r="F43">
-        <f t="shared" si="0"/>
+        <f>E43*O43</f>
         <v>621830.022</v>
       </c>
       <c r="G43">
         <v>53.960000000000001</v>
       </c>
       <c r="H43">
-        <f t="shared" si="1"/>
+        <f>G43*O43</f>
         <v>649012.53359999997</v>
       </c>
-      <c r="K43" t="s">
-        <v>16</v>
+      <c r="I43">
+        <v>50.321919712633878</v>
       </c>
       <c r="L43" t="s">
-        <v>16</v>
-      </c>
-      <c r="N43" s="5">
+        <v>17</v>
+      </c>
+      <c r="M43" t="s">
+        <v>17</v>
+      </c>
+      <c r="O43" s="5">
         <v>12027.66</v>
       </c>
-      <c r="O43">
+      <c r="P43">
         <v>0.25025967487183648</v>
       </c>
     </row>
@@ -2562,7 +2695,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C44">
         <v>51.859999999999999</v>
@@ -2574,26 +2707,29 @@
         <v>49.829999999999998</v>
       </c>
       <c r="F44">
-        <f t="shared" si="0"/>
+        <f>E44*O44</f>
         <v>595202.40779999993</v>
       </c>
       <c r="G44">
         <v>54.390000000000001</v>
       </c>
       <c r="H44">
-        <f t="shared" si="1"/>
+        <f>G44*O44</f>
         <v>649670.05740000005</v>
       </c>
-      <c r="K44" t="s">
-        <v>16</v>
+      <c r="I44">
+        <v>52.54483683140402</v>
       </c>
       <c r="L44" t="s">
-        <v>16</v>
-      </c>
-      <c r="N44" s="5">
+        <v>17</v>
+      </c>
+      <c r="M44" t="s">
+        <v>17</v>
+      </c>
+      <c r="O44" s="5">
         <v>11944.66</v>
       </c>
-      <c r="O44">
+      <c r="P44">
         <v>0.081081308556566506</v>
       </c>
     </row>
@@ -2602,7 +2738,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C45">
         <v>51.590000000000003</v>
@@ -2614,26 +2750,29 @@
         <v>46.350000000000001</v>
       </c>
       <c r="F45">
-        <f t="shared" si="0"/>
+        <f>E45*O45</f>
         <v>553391.18999999994</v>
       </c>
       <c r="G45">
         <v>53.380000000000003</v>
       </c>
       <c r="H45">
-        <f t="shared" si="1"/>
+        <f>G45*O45</f>
         <v>637325.17200000002</v>
       </c>
-      <c r="K45" t="s">
-        <v>16</v>
+      <c r="I45">
+        <v>53.415622515678912</v>
       </c>
       <c r="L45" t="s">
-        <v>16</v>
-      </c>
-      <c r="N45" s="5">
+        <v>17</v>
+      </c>
+      <c r="M45" t="s">
+        <v>17</v>
+      </c>
+      <c r="O45" s="5">
         <v>11939.4</v>
       </c>
-      <c r="O45">
+      <c r="P45">
         <v>0.13954677897903511</v>
       </c>
     </row>
@@ -2642,7 +2781,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C46">
         <v>51.969999999999999</v>
@@ -2654,26 +2793,29 @@
         <v>48.840000000000003</v>
       </c>
       <c r="F46">
-        <f t="shared" si="0"/>
+        <f>E46*O46</f>
         <v>582698.80680000002</v>
       </c>
       <c r="G46">
         <v>52.75</v>
       </c>
       <c r="H46">
-        <f t="shared" si="1"/>
+        <f>G46*O46</f>
         <v>629348.11750000005</v>
       </c>
-      <c r="K46" t="s">
-        <v>16</v>
+      <c r="I46">
+        <v>53.307849747685772</v>
       </c>
       <c r="L46" t="s">
-        <v>16</v>
-      </c>
-      <c r="N46" s="5">
+        <v>17</v>
+      </c>
+      <c r="M46" t="s">
+        <v>17</v>
+      </c>
+      <c r="O46" s="5">
         <v>11930.77</v>
       </c>
-      <c r="O46">
+      <c r="P46">
         <v>0.1607070528895688</v>
       </c>
     </row>
@@ -2682,7 +2824,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C47">
         <v>51.990000000000002</v>
@@ -2694,26 +2836,29 @@
         <v>50.600000000000001</v>
       </c>
       <c r="F47">
-        <f t="shared" si="0"/>
+        <f>E47*O47</f>
         <v>609130.89600000007</v>
       </c>
       <c r="G47">
         <v>54.640000000000001</v>
       </c>
       <c r="H47">
-        <f t="shared" si="1"/>
+        <f>G47*O47</f>
         <v>657765.06240000005</v>
       </c>
-      <c r="K47" t="s">
-        <v>16</v>
+      <c r="I47">
+        <v>55.983254561998073</v>
       </c>
       <c r="L47" t="s">
-        <v>16</v>
-      </c>
-      <c r="N47" s="5">
+        <v>17</v>
+      </c>
+      <c r="M47" t="s">
+        <v>17</v>
+      </c>
+      <c r="O47" s="5">
         <v>12038.16</v>
       </c>
-      <c r="O47">
+      <c r="P47">
         <v>0.26412440048150088</v>
       </c>
     </row>
@@ -2722,7 +2867,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C48">
         <v>51.810000000000002</v>
@@ -2734,26 +2879,29 @@
         <v>48.640000000000001</v>
       </c>
       <c r="F48">
-        <f t="shared" si="0"/>
+        <f>E48*O48</f>
         <v>580600.60160000005</v>
       </c>
       <c r="G48">
         <v>54.670000000000002</v>
       </c>
       <c r="H48">
-        <f t="shared" si="1"/>
+        <f>G48*O48</f>
         <v>652578.84230000002</v>
       </c>
-      <c r="K48" t="s">
-        <v>16</v>
+      <c r="I48">
+        <v>54.079736244886803</v>
       </c>
       <c r="L48" t="s">
-        <v>16</v>
-      </c>
-      <c r="N48" s="5">
+        <v>17</v>
+      </c>
+      <c r="M48" t="s">
+        <v>17</v>
+      </c>
+      <c r="O48" s="5">
         <v>11936.690000000001</v>
       </c>
-      <c r="O48">
+      <c r="P48">
         <v>0.32607479529505362</v>
       </c>
     </row>
@@ -2762,7 +2910,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C49">
         <v>52.07</v>
@@ -2774,26 +2922,29 @@
         <v>51.270000000000003</v>
       </c>
       <c r="F49">
-        <f t="shared" si="0"/>
+        <f>E49*O49</f>
         <v>602833.1727</v>
       </c>
       <c r="G49">
         <v>51.740000000000002</v>
       </c>
       <c r="H49">
-        <f t="shared" si="1"/>
+        <f>G49*O49</f>
         <v>608359.43740000005</v>
       </c>
-      <c r="K49" t="s">
-        <v>16</v>
+      <c r="I49">
+        <v>56.324988781882034</v>
       </c>
       <c r="L49" t="s">
-        <v>16</v>
-      </c>
-      <c r="N49" s="5">
+        <v>17</v>
+      </c>
+      <c r="M49" t="s">
+        <v>17</v>
+      </c>
+      <c r="O49" s="5">
         <v>11758.01</v>
       </c>
-      <c r="O49">
+      <c r="P49">
         <v>0.1114193728838956</v>
       </c>
     </row>
@@ -2802,7 +2953,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C50">
         <v>52.130000000000003</v>
@@ -2814,26 +2965,29 @@
         <v>50.189999999999998</v>
       </c>
       <c r="F50">
-        <f t="shared" si="0"/>
+        <f>E50*O50</f>
         <v>588505.85639999993</v>
       </c>
       <c r="G50">
         <v>55.189999999999998</v>
       </c>
       <c r="H50">
-        <f t="shared" si="1"/>
+        <f>G50*O50</f>
         <v>647133.65639999998</v>
       </c>
-      <c r="K50" t="s">
-        <v>16</v>
+      <c r="I50">
+        <v>61.907301004556473</v>
       </c>
       <c r="L50" t="s">
-        <v>16</v>
-      </c>
-      <c r="N50" s="5">
+        <v>17</v>
+      </c>
+      <c r="M50" t="s">
+        <v>17</v>
+      </c>
+      <c r="O50" s="5">
         <v>11725.559999999999</v>
       </c>
-      <c r="O50">
+      <c r="P50">
         <v>0.16331036630501561</v>
       </c>
     </row>
@@ -2842,7 +2996,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C51">
         <v>51.890000000000001</v>
@@ -2854,26 +3008,29 @@
         <v>47.539999999999999</v>
       </c>
       <c r="F51">
-        <f t="shared" si="0"/>
+        <f>E51*O51</f>
         <v>572851.29519999993</v>
       </c>
       <c r="G51">
         <v>55.759999999999998</v>
       </c>
       <c r="H51">
-        <f t="shared" si="1"/>
+        <f>G51*O51</f>
         <v>671901.30879999988</v>
       </c>
-      <c r="K51" t="s">
-        <v>16</v>
+      <c r="I51">
+        <v>51.124330876188566</v>
       </c>
       <c r="L51" t="s">
-        <v>16</v>
-      </c>
-      <c r="N51" s="5">
+        <v>17</v>
+      </c>
+      <c r="M51" t="s">
+        <v>17</v>
+      </c>
+      <c r="O51" s="5">
         <v>12049.879999999999</v>
       </c>
-      <c r="O51">
+      <c r="P51">
         <v>0.2499149953121034</v>
       </c>
     </row>
@@ -2882,7 +3039,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C52">
         <v>52</v>
@@ -2894,26 +3051,29 @@
         <v>49.590000000000003</v>
       </c>
       <c r="F52">
-        <f t="shared" si="0"/>
+        <f>E52*O52</f>
         <v>596212.63560000004</v>
       </c>
       <c r="G52">
         <v>55.149999999999999</v>
       </c>
       <c r="H52">
-        <f t="shared" si="1"/>
+        <f>G52*O52</f>
         <v>663059.62600000005</v>
       </c>
-      <c r="K52" t="s">
-        <v>16</v>
+      <c r="I52">
+        <v>57.660281137502921</v>
       </c>
       <c r="L52" t="s">
-        <v>16</v>
-      </c>
-      <c r="N52" s="5">
+        <v>17</v>
+      </c>
+      <c r="M52" t="s">
+        <v>17</v>
+      </c>
+      <c r="O52" s="5">
         <v>12022.84</v>
       </c>
-      <c r="O52">
+      <c r="P52">
         <v>0.27923866419586152</v>
       </c>
     </row>
@@ -2922,7 +3082,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C53">
         <v>52.409999999999997</v>
@@ -2934,26 +3094,29 @@
         <v>53.159999999999997</v>
       </c>
       <c r="F53">
-        <f t="shared" si="0"/>
+        <f>E53*O53</f>
         <v>644857.38</v>
       </c>
       <c r="G53">
         <v>53.899999999999999</v>
       </c>
       <c r="H53">
-        <f t="shared" si="1"/>
+        <f>G53*O53</f>
         <v>653833.94999999995</v>
       </c>
-      <c r="K53" t="s">
-        <v>16</v>
+      <c r="I53">
+        <v>52.095678031344448</v>
       </c>
       <c r="L53" t="s">
-        <v>16</v>
-      </c>
-      <c r="N53" s="5">
+        <v>17</v>
+      </c>
+      <c r="M53" t="s">
+        <v>17</v>
+      </c>
+      <c r="O53" s="5">
         <v>12130.5</v>
       </c>
-      <c r="O53">
+      <c r="P53">
         <v>0.26553641868929079</v>
       </c>
     </row>
@@ -2962,7 +3125,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C54">
         <v>51.869999999999997</v>
@@ -2974,26 +3137,29 @@
         <v>48.240000000000002</v>
       </c>
       <c r="F54">
-        <f t="shared" si="0"/>
+        <f>E54*O54</f>
         <v>581485.92480000004</v>
       </c>
       <c r="G54">
         <v>53.539999999999999</v>
       </c>
       <c r="H54">
-        <f t="shared" si="1"/>
+        <f>G54*O54</f>
         <v>645372.23080000002</v>
       </c>
-      <c r="K54" t="s">
-        <v>16</v>
+      <c r="I54">
+        <v>55.447233244750741</v>
       </c>
       <c r="L54" t="s">
-        <v>16</v>
-      </c>
-      <c r="N54" s="5">
+        <v>17</v>
+      </c>
+      <c r="M54" t="s">
+        <v>17</v>
+      </c>
+      <c r="O54" s="5">
         <v>12054.02</v>
       </c>
-      <c r="O54">
+      <c r="P54">
         <v>0.2101789961585728</v>
       </c>
     </row>
@@ -3002,7 +3168,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C55">
         <v>51.799999999999997</v>
@@ -3014,26 +3180,29 @@
         <v>48.509999999999998</v>
       </c>
       <c r="F55">
-        <f t="shared" si="0"/>
+        <f>E55*O55</f>
         <v>573418.7612999999</v>
       </c>
       <c r="G55">
         <v>51.770000000000003</v>
       </c>
       <c r="H55">
-        <f t="shared" si="1"/>
+        <f>G55*O55</f>
         <v>611954.01509999996</v>
       </c>
-      <c r="K55" t="s">
-        <v>16</v>
+      <c r="I55">
+        <v>65.85490215258379</v>
       </c>
       <c r="L55" t="s">
-        <v>16</v>
-      </c>
-      <c r="N55" s="5">
+        <v>17</v>
+      </c>
+      <c r="M55" t="s">
+        <v>17</v>
+      </c>
+      <c r="O55" s="5">
         <v>11820.629999999999</v>
       </c>
-      <c r="O55">
+      <c r="P55">
         <v>0.3924639985962457</v>
       </c>
     </row>
@@ -3042,7 +3211,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C56">
         <v>52.090000000000003</v>
@@ -3054,29 +3223,32 @@
         <v>50.829999999999998</v>
       </c>
       <c r="F56">
-        <f t="shared" si="0"/>
+        <f>E56*O56</f>
         <v>598923.79039999994</v>
       </c>
       <c r="G56">
         <v>51.210000000000001</v>
       </c>
       <c r="H56">
-        <f t="shared" si="1"/>
+        <f>G56*O56</f>
         <v>603401.28480000002</v>
       </c>
-      <c r="J56">
+      <c r="I56">
+        <v>73.319368116051592</v>
+      </c>
+      <c r="K56">
         <v>3383.2399999999998</v>
       </c>
-      <c r="K56" t="s">
-        <v>16</v>
-      </c>
       <c r="L56" t="s">
-        <v>16</v>
-      </c>
-      <c r="N56" s="5">
+        <v>17</v>
+      </c>
+      <c r="M56" t="s">
+        <v>17</v>
+      </c>
+      <c r="O56" s="5">
         <v>11782.879999999999</v>
       </c>
-      <c r="O56">
+      <c r="P56">
         <v>0.40754358832383869</v>
       </c>
     </row>
@@ -3085,7 +3257,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C57">
         <v>52.75</v>
@@ -3097,26 +3269,29 @@
         <v>57.170000000000002</v>
       </c>
       <c r="F57">
-        <f t="shared" si="0"/>
+        <f>E57*O57</f>
         <v>691288.20600000001</v>
       </c>
       <c r="G57">
         <v>54.030000000000001</v>
       </c>
       <c r="H57">
-        <f t="shared" si="1"/>
+        <f>G57*O57</f>
         <v>653319.95400000003</v>
       </c>
-      <c r="K57" t="s">
-        <v>16</v>
+      <c r="I57">
+        <v>65.681300965259666</v>
       </c>
       <c r="L57" t="s">
-        <v>16</v>
-      </c>
-      <c r="N57" s="5">
+        <v>17</v>
+      </c>
+      <c r="M57" t="s">
+        <v>17</v>
+      </c>
+      <c r="O57" s="5">
         <v>12091.799999999999</v>
       </c>
-      <c r="O57">
+      <c r="P57">
         <v>0.27516496832785431</v>
       </c>
     </row>
@@ -3125,7 +3300,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C58">
         <v>52.020000000000003</v>
@@ -3137,29 +3312,32 @@
         <v>49.93</v>
       </c>
       <c r="F58">
-        <f t="shared" si="0"/>
+        <f>E58*O58</f>
         <v>600369.30459999992</v>
       </c>
       <c r="G58">
         <v>53.969999999999999</v>
       </c>
       <c r="H58">
-        <f t="shared" si="1"/>
+        <f>G58*O58</f>
         <v>648947.15339999995</v>
       </c>
-      <c r="J58">
+      <c r="I58">
+        <v>55.367386294088902</v>
+      </c>
+      <c r="K58">
         <v>2109.5700000000002</v>
       </c>
-      <c r="K58" t="s">
-        <v>16</v>
-      </c>
       <c r="L58" t="s">
-        <v>16</v>
-      </c>
-      <c r="N58" s="5">
+        <v>17</v>
+      </c>
+      <c r="M58" t="s">
+        <v>17</v>
+      </c>
+      <c r="O58" s="5">
         <v>12024.219999999999</v>
       </c>
-      <c r="O58">
+      <c r="P58">
         <v>0.14460868624103909</v>
       </c>
     </row>
@@ -3168,7 +3346,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C59">
         <v>50.859999999999999</v>
@@ -3180,29 +3358,32 @@
         <v>43.520000000000003</v>
       </c>
       <c r="F59">
-        <f t="shared" si="0"/>
+        <f>E59*O59</f>
         <v>515237.19680000003</v>
       </c>
       <c r="G59">
         <v>56.25</v>
       </c>
       <c r="H59">
-        <f t="shared" si="1"/>
+        <f>G59*O59</f>
         <v>665948.8125</v>
       </c>
-      <c r="J59" t="s">
-        <v>17</v>
+      <c r="I59">
+        <v>54.752281050039173</v>
       </c>
       <c r="K59" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L59" t="s">
-        <v>16</v>
-      </c>
-      <c r="N59" s="5">
+        <v>17</v>
+      </c>
+      <c r="M59" t="s">
+        <v>17</v>
+      </c>
+      <c r="O59" s="5">
         <v>11839.09</v>
       </c>
-      <c r="O59">
+      <c r="P59">
         <v>0.27097259435514548</v>
       </c>
     </row>
@@ -3211,7 +3392,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C60">
         <v>52.18</v>
@@ -3223,29 +3404,32 @@
         <v>49.82</v>
       </c>
       <c r="F60">
-        <f t="shared" si="0"/>
+        <f>E60*O60</f>
         <v>596217.36259999999</v>
       </c>
       <c r="G60">
         <v>55.359999999999999</v>
       </c>
       <c r="H60">
-        <f t="shared" si="1"/>
+        <f>G60*O60</f>
         <v>662516.92480000004</v>
       </c>
-      <c r="J60">
+      <c r="I60">
+        <v>61.243807380404157</v>
+      </c>
+      <c r="K60">
         <v>2905.27</v>
       </c>
-      <c r="K60" t="s">
-        <v>16</v>
-      </c>
       <c r="L60" t="s">
-        <v>16</v>
-      </c>
-      <c r="N60" s="5">
+        <v>17</v>
+      </c>
+      <c r="M60" t="s">
+        <v>17</v>
+      </c>
+      <c r="O60" s="5">
         <v>11967.43</v>
       </c>
-      <c r="O60">
+      <c r="P60">
         <v>0.35552049467337099</v>
       </c>
     </row>
@@ -3254,7 +3438,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C61">
         <v>52.159999999999997</v>
@@ -3266,29 +3450,32 @@
         <v>51.600000000000001</v>
       </c>
       <c r="F61">
-        <f t="shared" si="0"/>
+        <f>E61*O61</f>
         <v>621969.88800000004</v>
       </c>
       <c r="G61">
         <v>53.25</v>
       </c>
       <c r="H61">
-        <f t="shared" si="1"/>
+        <f>G61*O61</f>
         <v>641858.45999999996</v>
       </c>
-      <c r="J61">
+      <c r="I61">
+        <v>55.867138071399843</v>
+      </c>
+      <c r="K61">
         <v>1808.48</v>
       </c>
-      <c r="K61" t="s">
-        <v>16</v>
-      </c>
       <c r="L61" t="s">
-        <v>16</v>
-      </c>
-      <c r="N61" s="5">
+        <v>17</v>
+      </c>
+      <c r="M61" t="s">
+        <v>17</v>
+      </c>
+      <c r="O61" s="5">
         <v>12053.68</v>
       </c>
-      <c r="O61">
+      <c r="P61">
         <v>0.36673432173800208</v>
       </c>
     </row>
@@ -3297,7 +3484,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C62">
         <v>51.5</v>
@@ -3309,29 +3496,32 @@
         <v>46.469999999999999</v>
       </c>
       <c r="F62">
-        <f t="shared" si="0"/>
+        <f>E62*O62</f>
         <v>557712.95789999992</v>
       </c>
       <c r="G62">
         <v>52.619999999999997</v>
       </c>
       <c r="H62">
-        <f t="shared" si="1"/>
+        <f>G62*O62</f>
         <v>631522.61339999991</v>
       </c>
-      <c r="J62">
+      <c r="I62">
+        <v>71.612220860983854</v>
+      </c>
+      <c r="K62">
         <v>1789.1199999999999</v>
       </c>
-      <c r="K62" t="s">
-        <v>16</v>
-      </c>
       <c r="L62" t="s">
-        <v>16</v>
-      </c>
-      <c r="N62" s="5">
+        <v>17</v>
+      </c>
+      <c r="M62" t="s">
+        <v>17</v>
+      </c>
+      <c r="O62" s="5">
         <v>12001.57</v>
       </c>
-      <c r="O62">
+      <c r="P62">
         <v>0.47577011580580458</v>
       </c>
     </row>
@@ -3340,7 +3530,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C63">
         <v>51.399999999999999</v>
@@ -3352,29 +3542,32 @@
         <v>46.520000000000003</v>
       </c>
       <c r="F63">
-        <f t="shared" si="0"/>
+        <f>E63*O63</f>
         <v>566467.52720000001</v>
       </c>
       <c r="G63">
         <v>54.490000000000002</v>
       </c>
       <c r="H63">
-        <f t="shared" si="1"/>
+        <f>G63*O63</f>
         <v>663517.10140000004</v>
       </c>
-      <c r="J63">
+      <c r="I63">
+        <v>67.098116212605291</v>
+      </c>
+      <c r="K63">
         <v>1622.77</v>
       </c>
-      <c r="K63" t="s">
-        <v>16</v>
-      </c>
       <c r="L63" t="s">
-        <v>16</v>
-      </c>
-      <c r="N63" s="5">
+        <v>17</v>
+      </c>
+      <c r="M63" t="s">
+        <v>17</v>
+      </c>
+      <c r="O63" s="5">
         <v>12176.860000000001</v>
       </c>
-      <c r="O63">
+      <c r="P63">
         <v>0.53245573334480567</v>
       </c>
     </row>
@@ -3383,7 +3576,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C64">
         <v>51.25</v>
@@ -3395,29 +3588,32 @@
         <v>45.229999999999997</v>
       </c>
       <c r="F64">
-        <f t="shared" si="0"/>
+        <f>E64*O64</f>
         <v>542328.50579999993</v>
       </c>
       <c r="G64">
         <v>55.369999999999997</v>
       </c>
       <c r="H64">
-        <f t="shared" si="1"/>
+        <f>G64*O64</f>
         <v>663911.77019999991</v>
       </c>
-      <c r="J64">
+      <c r="I64">
+        <v>56.370761535266901</v>
+      </c>
+      <c r="K64">
         <v>1730.8</v>
       </c>
-      <c r="K64" t="s">
-        <v>16</v>
-      </c>
       <c r="L64" t="s">
-        <v>16</v>
-      </c>
-      <c r="N64" s="5">
+        <v>17</v>
+      </c>
+      <c r="M64" t="s">
+        <v>17</v>
+      </c>
+      <c r="O64" s="5">
         <v>11990.459999999999</v>
       </c>
-      <c r="O64">
+      <c r="P64">
         <v>0.38645735255535968</v>
       </c>
     </row>
@@ -3426,7 +3622,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C65">
         <v>50.590000000000003</v>
@@ -3438,29 +3634,32 @@
         <v>47.170000000000002</v>
       </c>
       <c r="F65">
-        <f t="shared" si="0"/>
+        <f>E65*O65</f>
         <v>572022.57110000006</v>
       </c>
       <c r="G65">
         <v>54.880000000000003</v>
       </c>
       <c r="H65">
-        <f t="shared" si="1"/>
+        <f>G65*O65</f>
         <v>665520.43040000007</v>
       </c>
-      <c r="J65" t="s">
-        <v>17</v>
+      <c r="I65">
+        <v>61.894312878109993</v>
       </c>
       <c r="K65" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L65" t="s">
-        <v>16</v>
-      </c>
-      <c r="N65" s="6">
+        <v>17</v>
+      </c>
+      <c r="M65" t="s">
+        <v>17</v>
+      </c>
+      <c r="O65" s="6">
         <v>12126.83</v>
       </c>
-      <c r="O65">
+      <c r="P65">
         <v>0.21921221517343861</v>
       </c>
     </row>

</xml_diff>